<commit_message>
changes to feature branch
</commit_message>
<xml_diff>
--- a/Custom Office Templates/Details of the Websites.xlsx
+++ b/Custom Office Templates/Details of the Websites.xlsx
@@ -19,9 +19,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Name</t>
+  </si>
+  <si>
+    <t>Lab 9</t>
+  </si>
+  <si>
+    <t>Lab 12</t>
+  </si>
+  <si>
+    <t>Lab 13</t>
+  </si>
+  <si>
+    <t>Lab 14</t>
   </si>
 </sst>
 </file>
@@ -403,10 +415,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.875" defaultRowHeight="21.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -419,6 +431,26 @@
         <v>0</v>
       </c>
     </row>
+    <row r="2" spans="1:1" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
final added in the worksheet
</commit_message>
<xml_diff>
--- a/Custom Office Templates/Details of the Websites.xlsx
+++ b/Custom Office Templates/Details of the Websites.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Name</t>
   </si>
@@ -34,6 +34,9 @@
   </si>
   <si>
     <t>Lab 14</t>
+  </si>
+  <si>
+    <t>final</t>
   </si>
 </sst>
 </file>
@@ -415,7 +418,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
@@ -451,6 +454,11 @@
         <v>4</v>
       </c>
     </row>
+    <row r="6" spans="1:1" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>